<commit_message>
removed models from git and added them to gitignore.  Fixed spelling mistake in mcc calc sheet
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobby\Desktop\CMSC435-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zephy\OneDrive\Documents\CMSC435-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17672" windowHeight="5852" xr2:uid="{F2834071-C162-40F0-9C47-59C1C10E8D85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17670" windowHeight="5850" xr2:uid="{F2834071-C162-40F0-9C47-59C1C10E8D85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Quality Measure</t>
   </si>
   <si>
-    <t>Sentsitivity</t>
-  </si>
-  <si>
     <t>Specificity</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>SVM</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
   </si>
 </sst>
 </file>
@@ -481,18 +481,18 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" customWidth="1"/>
-    <col min="6" max="6" width="14.8984375" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -500,144 +500,144 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C2" s="9">
         <v>78.2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="9">
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="9">
         <v>74.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6">
         <v>0.44900000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9">
         <v>90.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="9">
         <v>26.8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="9">
         <v>77.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6">
         <v>0.19900000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9">
         <v>86.2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="9">
         <v>46.6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="9">
         <v>81.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6">
         <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9">
         <v>61</v>
@@ -658,10 +658,10 @@
         <v>34.966777408637874</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="9">
         <v>83.6</v>
@@ -682,10 +682,10 @@
         <v>90.306336550566513</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="9">
         <v>76.099999999999994</v>
@@ -706,10 +706,10 @@
         <v>71.731251742403117</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="6">
         <v>0.45500000000000002</v>
@@ -730,9 +730,9 @@
         <v>0.3094611746013306</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6">
         <f>AVERAGE(C5,C9,C13,C17)</f>
@@ -747,9 +747,9 @@
         <v>0.25977591745097944</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>